<commit_message>
Update files and fix bugs
</commit_message>
<xml_diff>
--- a/Test Files/Alt Index - Initial.xlsx
+++ b/Test Files/Alt Index - Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C46424-CEB3-42EC-9BFD-926753873D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C92FED-D132-4CE2-A499-714E810FF729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2805" windowWidth="17580" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5175" yWindow="3570" windowWidth="17580" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>AltIndex-A</t>
   </si>
@@ -101,66 +101,6 @@
     <t>bad</t>
   </si>
   <si>
-    <t>R-201-I1-CS1-0E75</t>
-  </si>
-  <si>
-    <t>R-202-I2-Cb1-4E5E</t>
-  </si>
-  <si>
-    <t>R-203-I3-CS2-F8F3</t>
-  </si>
-  <si>
-    <t>R-204-I4-Cf1-CF85</t>
-  </si>
-  <si>
-    <t>R-205-I5-Ce1-7574</t>
-  </si>
-  <si>
-    <t>R-206-I6-CT1-77AF</t>
-  </si>
-  <si>
-    <t>R-207-I7-CE2-CF6A</t>
-  </si>
-  <si>
-    <t>R-208-I8-CS1-BB53</t>
-  </si>
-  <si>
-    <t>R-209-I9-Cb1-581E</t>
-  </si>
-  <si>
-    <t>R-210-I10-CS2-5050</t>
-  </si>
-  <si>
-    <t>R-211-I11-Cf1-3615</t>
-  </si>
-  <si>
-    <t>R-212-I12-Ce1-5F24</t>
-  </si>
-  <si>
-    <t>R-213-I13-CT1-C5C9</t>
-  </si>
-  <si>
-    <t>R-214-I14-CE2-D2F0</t>
-  </si>
-  <si>
-    <t>R-215-I15-CS1-498E</t>
-  </si>
-  <si>
-    <t>R-216-I16-Cb1-B7F7</t>
-  </si>
-  <si>
-    <t>R-217-I17-CS2-50A6</t>
-  </si>
-  <si>
-    <t>R-218-I18-Cf1-20D8</t>
-  </si>
-  <si>
-    <t>R-219-I19-Ce1-4D3C</t>
-  </si>
-  <si>
-    <t>R-220-I20-CT1-A141</t>
-  </si>
-  <si>
     <t>normal</t>
   </si>
   <si>
@@ -171,6 +111,72 @@
   </si>
   <si>
     <t>Engine</t>
+  </si>
+  <si>
+    <t>R-222-I22-CS2-7D79</t>
+  </si>
+  <si>
+    <t>R-211-I11-Cf1-9B8C</t>
+  </si>
+  <si>
+    <t>R-212-I12-Ce1-2186</t>
+  </si>
+  <si>
+    <t>R-203-I3-CS2-7A3F</t>
+  </si>
+  <si>
+    <t>R-208-I8-CS1-22BF</t>
+  </si>
+  <si>
+    <t>R-209-I9-Cb1-6694</t>
+  </si>
+  <si>
+    <t>R-215-I15-CS1-96FB</t>
+  </si>
+  <si>
+    <t>R-210-I10-CS2-BD7D</t>
+  </si>
+  <si>
+    <t>R-219-I19-Ce1-922D</t>
+  </si>
+  <si>
+    <t>R-202-I2-Cb1-8C22</t>
+  </si>
+  <si>
+    <t>R-213-I13-CT1-A74F</t>
+  </si>
+  <si>
+    <t>R-204-I4-Cf1-3967</t>
+  </si>
+  <si>
+    <t>R-207-I7-CE2-4D7F</t>
+  </si>
+  <si>
+    <t>R-217-I17-CS2-96CC</t>
+  </si>
+  <si>
+    <t>R-201-I1-CS1-674B</t>
+  </si>
+  <si>
+    <t>R-218-I18-Cf1-E368</t>
+  </si>
+  <si>
+    <t>R-206-I6-CT1-012B</t>
+  </si>
+  <si>
+    <t>R-220-I20-CT1-C738</t>
+  </si>
+  <si>
+    <t>R-216-I16-Cb1-F7E7</t>
+  </si>
+  <si>
+    <t>R-205-I5-Ce1-236C</t>
+  </si>
+  <si>
+    <t>R-214-I14-CE2-CF3C</t>
+  </si>
+  <si>
+    <t>AltIndex-V</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -591,7 +597,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -605,43 +611,43 @@
         <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C21" si="0">5*ROW()</f>
+        <f t="shared" ref="C3:C22" si="0">5*ROW()</f>
         <v>15</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" si="1">100*ROW()</f>
+        <f t="shared" ref="D3:D22" si="1">100*ROW()</f>
         <v>300</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -655,18 +661,18 @@
         <v>400</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -680,18 +686,18 @@
         <v>500</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -705,18 +711,18 @@
         <v>600</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -730,18 +736,18 @@
         <v>700</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -755,18 +761,18 @@
         <v>800</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -780,18 +786,18 @@
         <v>900</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -805,18 +811,18 @@
         <v>1000</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -836,12 +842,12 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -855,18 +861,18 @@
         <v>1200</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -886,12 +892,12 @@
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -905,18 +911,18 @@
         <v>1400</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -936,12 +942,12 @@
         <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -955,18 +961,18 @@
         <v>1600</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -986,12 +992,12 @@
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1005,18 +1011,18 @@
         <v>1800</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1036,12 +1042,12 @@
         <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1055,18 +1061,18 @@
         <v>2000</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -1080,13 +1086,38 @@
         <v>2100</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <f>5*ROW()</f>
+        <v>110</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix import functionality and add newAltIndexToAdd array
</commit_message>
<xml_diff>
--- a/Test Files/Alt Index - Initial.xlsx
+++ b/Test Files/Alt Index - Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C92FED-D132-4CE2-A499-714E810FF729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04488FF7-1EF6-4E6C-A397-C1935A6C7E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="3570" windowWidth="17580" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="3165" windowWidth="17580" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -113,70 +113,70 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>R-222-I22-CS2-7D79</t>
-  </si>
-  <si>
-    <t>R-211-I11-Cf1-9B8C</t>
-  </si>
-  <si>
-    <t>R-212-I12-Ce1-2186</t>
-  </si>
-  <si>
-    <t>R-203-I3-CS2-7A3F</t>
-  </si>
-  <si>
-    <t>R-208-I8-CS1-22BF</t>
-  </si>
-  <si>
-    <t>R-209-I9-Cb1-6694</t>
-  </si>
-  <si>
-    <t>R-215-I15-CS1-96FB</t>
-  </si>
-  <si>
-    <t>R-210-I10-CS2-BD7D</t>
-  </si>
-  <si>
-    <t>R-219-I19-Ce1-922D</t>
-  </si>
-  <si>
-    <t>R-202-I2-Cb1-8C22</t>
-  </si>
-  <si>
-    <t>R-213-I13-CT1-A74F</t>
-  </si>
-  <si>
-    <t>R-204-I4-Cf1-3967</t>
-  </si>
-  <si>
-    <t>R-207-I7-CE2-4D7F</t>
-  </si>
-  <si>
-    <t>R-217-I17-CS2-96CC</t>
-  </si>
-  <si>
-    <t>R-201-I1-CS1-674B</t>
-  </si>
-  <si>
-    <t>R-218-I18-Cf1-E368</t>
-  </si>
-  <si>
-    <t>R-206-I6-CT1-012B</t>
-  </si>
-  <si>
-    <t>R-220-I20-CT1-C738</t>
-  </si>
-  <si>
-    <t>R-216-I16-Cb1-F7E7</t>
-  </si>
-  <si>
-    <t>R-205-I5-Ce1-236C</t>
-  </si>
-  <si>
-    <t>R-214-I14-CE2-CF3C</t>
-  </si>
-  <si>
     <t>AltIndex-V</t>
+  </si>
+  <si>
+    <t>R-201-I1-CS1-7B4D</t>
+  </si>
+  <si>
+    <t>R-202-I2-Cb1-F317</t>
+  </si>
+  <si>
+    <t>R-203-I3-CS2-5B61</t>
+  </si>
+  <si>
+    <t>R-204-I4-Cf1-62A0</t>
+  </si>
+  <si>
+    <t>R-205-I5-Ce1-4C99</t>
+  </si>
+  <si>
+    <t>R-206-I6-CT1-64E3</t>
+  </si>
+  <si>
+    <t>R-207-I7-CE2-9616</t>
+  </si>
+  <si>
+    <t>R-208-I8-CS1-D002</t>
+  </si>
+  <si>
+    <t>R-209-I9-Cb1-0D0C</t>
+  </si>
+  <si>
+    <t>R-210-I10-CS2-8217</t>
+  </si>
+  <si>
+    <t>R-211-I11-Cf1-ACC5</t>
+  </si>
+  <si>
+    <t>R-212-I12-Ce1-00F4</t>
+  </si>
+  <si>
+    <t>R-213-I13-CT1-B5AB</t>
+  </si>
+  <si>
+    <t>R-214-I14-CE2-1A71</t>
+  </si>
+  <si>
+    <t>R-215-I15-CS1-4111</t>
+  </si>
+  <si>
+    <t>R-216-I16-Cb1-7510</t>
+  </si>
+  <si>
+    <t>R-217-I17-CS2-942F</t>
+  </si>
+  <si>
+    <t>R-218-I18-Cf1-AE28</t>
+  </si>
+  <si>
+    <t>R-219-I19-Ce1-8FFF</t>
+  </si>
+  <si>
+    <t>R-220-I20-CT1-6919</t>
+  </si>
+  <si>
+    <t>R-222-I22-CS2-06EC</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -597,7 +597,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -622,13 +622,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="0">5*ROW()</f>
+        <f t="shared" ref="C3:C21" si="0">5*ROW()</f>
         <v>15</v>
       </c>
       <c r="D3">
@@ -672,7 +672,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -1097,10 +1097,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
         <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
       </c>
       <c r="C22">
         <f>5*ROW()</f>

</xml_diff>